<commit_message>
Finish training SA, ATE, ABSA using BERT on SemEval16 Restaurants and MAMS ATE
</commit_message>
<xml_diff>
--- a/results/ATE/SemEval16 - Task 5 - Restaurants/ATE_SemEval16_Results.xlsx
+++ b/results/ATE/SemEval16 - Task 5 - Restaurants/ATE_SemEval16_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\absa-online-reviews\results\ATE\SemEval16 - Task 5 - Restaurants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111EE49C-9F5B-4A96-A9C5-D38FE2BE5765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF27AD1-D376-4607-8537-BED5511A78FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="768" xr2:uid="{2BB8F1D5-1F1F-40BC-8E04-B3E7A6D9C2E3}"/>
+    <workbookView xWindow="5505" yWindow="3705" windowWidth="23295" windowHeight="11775" tabRatio="768" firstSheet="3" activeTab="4" xr2:uid="{2BB8F1D5-1F1F-40BC-8E04-B3E7A6D9C2E3}"/>
   </bookViews>
   <sheets>
     <sheet name="BERT ft+DO+CNN+BiLSTM+Linear" sheetId="10" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="30">
   <si>
     <t>Dataset:</t>
   </si>
@@ -48,19 +48,10 @@
     <t>Model:</t>
   </si>
   <si>
-    <t>Classes</t>
-  </si>
-  <si>
-    <t>positive, negative, neutral</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fine tuned BERT: </t>
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>Used only the sentences that contained only positive, negative or neutral labels (not mixed sentiments)</t>
   </si>
   <si>
     <t>Train batch size</t>
@@ -102,25 +93,7 @@
     <t>StdDev</t>
   </si>
   <si>
-    <t>BERT pretrained + Dropout + Linear - multi-class (positive, negative, neutral)</t>
-  </si>
-  <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>BERT finetuned + Dropout + Linear - multi-class (positive, negative, neutral)</t>
-  </si>
-  <si>
-    <t>BERT pretrained + Dropout + BiLSTM + Linear - multi-class (positive, negative, neutral)</t>
-  </si>
-  <si>
-    <t>BERT finetuned + Dropout + BiLSTM + Linear - multi-class (positive, negative, neutral)</t>
-  </si>
-  <si>
-    <t>BERT pretrained + Dropout + CNN + BiLSTM + Linear - multi-class (positive, negative, neutral)</t>
-  </si>
-  <si>
-    <t>BERT finetuned + Dropout + CNN + BiLSTM + Linear - multi-class (positive, negative, neutral)</t>
   </si>
   <si>
     <t>RTX 2060 SUPER</t>
@@ -133,6 +106,27 @@
   </si>
   <si>
     <t>8 GB</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>BERT pretrained + Dropout + Linear</t>
+  </si>
+  <si>
+    <t>BERT finetuned + Dropout + CNN + BiLSTM + Linear</t>
+  </si>
+  <si>
+    <t>BERT pretrained + Dropout + CNN + BiLSTM + Linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BERT finetuned + Dropout + BiLSTM + Linear </t>
+  </si>
+  <si>
+    <t>BERT pretrained + Dropout + BiLSTM + Linear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BERT finetuned + Dropout + Linear </t>
   </si>
 </sst>
 </file>
@@ -160,7 +154,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -594,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4CC195-E080-447C-8F25-04CD0A4744BB}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +624,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -638,37 +632,33 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -686,15 +676,16 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -707,7 +698,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -720,7 +711,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -742,31 +733,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -774,28 +765,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="10">
-        <v>0.99518799999999996</v>
+        <v>0.99494899999999997</v>
       </c>
       <c r="D14" s="10">
-        <v>0.99518799999999996</v>
+        <v>0.99494899999999997</v>
       </c>
       <c r="E14" s="10">
-        <v>0.631969</v>
+        <v>0.62029800000000002</v>
       </c>
       <c r="F14" s="10">
-        <v>0.99518799999999996</v>
+        <v>0.99494899999999997</v>
       </c>
       <c r="G14" s="10">
-        <v>0.35330400000000001</v>
+        <v>0.36418299999999998</v>
       </c>
       <c r="H14" s="10">
-        <v>0.99518799999999996</v>
+        <v>0.99494899999999997</v>
       </c>
       <c r="I14" s="10">
-        <v>0.36971900000000002</v>
+        <v>0.38766099999999998</v>
       </c>
       <c r="J14" s="10">
-        <v>363.68962900000002</v>
+        <v>364.73229600000002</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -803,28 +794,28 @@
         <v>2</v>
       </c>
       <c r="C15" s="10">
-        <v>0.99535899999999999</v>
+        <v>0.99492599999999998</v>
       </c>
       <c r="D15" s="10">
-        <v>0.99535899999999999</v>
+        <v>0.99492599999999998</v>
       </c>
       <c r="E15" s="10">
-        <v>0.61914000000000002</v>
+        <v>0.45904600000000001</v>
       </c>
       <c r="F15" s="10">
-        <v>0.99535899999999999</v>
+        <v>0.99492599999999998</v>
       </c>
       <c r="G15" s="10">
-        <v>0.37296800000000002</v>
+        <v>0.35664600000000002</v>
       </c>
       <c r="H15" s="10">
-        <v>0.99535899999999999</v>
+        <v>0.99492599999999998</v>
       </c>
       <c r="I15" s="10">
-        <v>0.40228900000000001</v>
+        <v>0.372002</v>
       </c>
       <c r="J15" s="10">
-        <v>360.75926900000002</v>
+        <v>361.31913900000001</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -832,28 +823,28 @@
         <v>3</v>
       </c>
       <c r="C16" s="10">
-        <v>0.99496899999999999</v>
+        <v>0.99520299999999995</v>
       </c>
       <c r="D16" s="10">
-        <v>0.99496899999999999</v>
+        <v>0.99520299999999995</v>
       </c>
       <c r="E16" s="10">
-        <v>0.64392000000000005</v>
+        <v>0.74086099999999999</v>
       </c>
       <c r="F16" s="10">
-        <v>0.99496899999999999</v>
+        <v>0.99520299999999995</v>
       </c>
       <c r="G16" s="10">
-        <v>0.36602400000000002</v>
+        <v>0.348298</v>
       </c>
       <c r="H16" s="10">
-        <v>0.99496899999999999</v>
+        <v>0.99520299999999995</v>
       </c>
       <c r="I16" s="10">
-        <v>0.39037699999999997</v>
+        <v>0.361377</v>
       </c>
       <c r="J16" s="10">
-        <v>360.192474</v>
+        <v>361.29593399999999</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -861,28 +852,28 @@
         <v>4</v>
       </c>
       <c r="C17" s="10">
-        <v>0.99522699999999997</v>
+        <v>0.99517199999999995</v>
       </c>
       <c r="D17" s="10">
-        <v>0.99522699999999997</v>
+        <v>0.99517199999999995</v>
       </c>
       <c r="E17" s="10">
-        <v>0.53263700000000003</v>
+        <v>0.45078299999999999</v>
       </c>
       <c r="F17" s="10">
-        <v>0.99522699999999997</v>
+        <v>0.99517199999999995</v>
       </c>
       <c r="G17" s="10">
-        <v>0.36497200000000002</v>
+        <v>0.33528400000000003</v>
       </c>
       <c r="H17" s="10">
-        <v>0.99522699999999997</v>
+        <v>0.99517199999999995</v>
       </c>
       <c r="I17" s="10">
-        <v>0.38427</v>
+        <v>0.33638200000000001</v>
       </c>
       <c r="J17" s="10">
-        <v>368.18672600000002</v>
+        <v>360.37720200000001</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -890,28 +881,28 @@
         <v>5</v>
       </c>
       <c r="C18" s="10">
-        <v>0.99555899999999997</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="D18" s="10">
-        <v>0.99555899999999997</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="E18" s="10">
-        <v>0.71349700000000005</v>
+        <v>0.582125</v>
       </c>
       <c r="F18" s="10">
-        <v>0.99555899999999997</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="G18" s="10">
-        <v>0.39868999999999999</v>
+        <v>0.36992000000000003</v>
       </c>
       <c r="H18" s="10">
-        <v>0.99555899999999997</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="I18" s="10">
-        <v>0.429373</v>
+        <v>0.392177</v>
       </c>
       <c r="J18" s="10">
-        <v>377.635806</v>
+        <v>360.619777</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -919,28 +910,28 @@
         <v>6</v>
       </c>
       <c r="C19" s="10">
-        <v>0.99531599999999998</v>
+        <v>0.99493799999999999</v>
       </c>
       <c r="D19" s="10">
-        <v>0.99531599999999998</v>
+        <v>0.99493799999999999</v>
       </c>
       <c r="E19" s="10">
-        <v>0.62787599999999999</v>
+        <v>0.54274</v>
       </c>
       <c r="F19" s="10">
-        <v>0.99531599999999998</v>
+        <v>0.99493799999999999</v>
       </c>
       <c r="G19" s="10">
-        <v>0.37391200000000002</v>
+        <v>0.34850799999999998</v>
       </c>
       <c r="H19" s="10">
-        <v>0.99531599999999998</v>
+        <v>0.99493799999999999</v>
       </c>
       <c r="I19" s="10">
-        <v>0.40155099999999999</v>
+        <v>0.36077999999999999</v>
       </c>
       <c r="J19" s="10">
-        <v>384.24440199999998</v>
+        <v>360.77993300000003</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -948,28 +939,28 @@
         <v>7</v>
       </c>
       <c r="C20" s="10">
-        <v>0.99493399999999999</v>
+        <v>0.995008</v>
       </c>
       <c r="D20" s="10">
-        <v>0.99493399999999999</v>
+        <v>0.995008</v>
       </c>
       <c r="E20" s="10">
-        <v>0.33164700000000003</v>
+        <v>0.455764</v>
       </c>
       <c r="F20" s="10">
-        <v>0.99493399999999999</v>
+        <v>0.995008</v>
       </c>
       <c r="G20" s="10">
-        <v>0.33333200000000002</v>
+        <v>0.36865999999999999</v>
       </c>
       <c r="H20" s="10">
-        <v>0.99493399999999999</v>
+        <v>0.995008</v>
       </c>
       <c r="I20" s="10">
-        <v>0.33248699999999998</v>
+        <v>0.38764399999999999</v>
       </c>
       <c r="J20" s="10">
-        <v>361.65589399999999</v>
+        <v>360.82172800000001</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -977,28 +968,28 @@
         <v>8</v>
       </c>
       <c r="C21" s="10">
-        <v>0.99470700000000001</v>
+        <v>0.99471100000000001</v>
       </c>
       <c r="D21" s="10">
-        <v>0.99470700000000001</v>
+        <v>0.99471100000000001</v>
       </c>
       <c r="E21" s="10">
-        <v>0.55131300000000005</v>
+        <v>0.45221499999999998</v>
       </c>
       <c r="F21" s="10">
-        <v>0.99470700000000001</v>
+        <v>0.99471100000000001</v>
       </c>
       <c r="G21" s="10">
-        <v>0.38498399999999999</v>
+        <v>0.34537699999999999</v>
       </c>
       <c r="H21" s="10">
-        <v>0.99470700000000001</v>
+        <v>0.99471100000000001</v>
       </c>
       <c r="I21" s="10">
-        <v>0.40923900000000002</v>
+        <v>0.35441800000000001</v>
       </c>
       <c r="J21" s="10">
-        <v>361.00166200000001</v>
+        <v>362.20333199999999</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1006,28 +997,28 @@
         <v>9</v>
       </c>
       <c r="C22" s="10">
-        <v>0.99495699999999998</v>
+        <v>0.99490999999999996</v>
       </c>
       <c r="D22" s="10">
-        <v>0.99495699999999998</v>
+        <v>0.99490999999999996</v>
       </c>
       <c r="E22" s="10">
-        <v>0.49842500000000001</v>
+        <v>0.52080300000000002</v>
       </c>
       <c r="F22" s="10">
-        <v>0.99495699999999998</v>
+        <v>0.99490999999999996</v>
       </c>
       <c r="G22" s="10">
-        <v>0.36266399999999999</v>
+        <v>0.359041</v>
       </c>
       <c r="H22" s="10">
-        <v>0.99495699999999998</v>
+        <v>0.99490999999999996</v>
       </c>
       <c r="I22" s="10">
-        <v>0.38248300000000002</v>
+        <v>0.37559399999999998</v>
       </c>
       <c r="J22" s="10">
-        <v>360.93821300000002</v>
+        <v>365.87313499999999</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -1035,28 +1026,28 @@
         <v>10</v>
       </c>
       <c r="C23" s="10">
-        <v>0.99498399999999998</v>
+        <v>0.99510200000000004</v>
       </c>
       <c r="D23" s="10">
-        <v>0.99498399999999998</v>
+        <v>0.99510200000000004</v>
       </c>
       <c r="E23" s="10">
-        <v>0.33166099999999998</v>
+        <v>0.46076299999999998</v>
       </c>
       <c r="F23" s="10">
-        <v>0.99498399999999998</v>
+        <v>0.99510200000000004</v>
       </c>
       <c r="G23" s="10">
-        <v>0.33333299999999999</v>
+        <v>0.35389100000000001</v>
       </c>
       <c r="H23" s="10">
-        <v>0.99498399999999998</v>
+        <v>0.99510200000000004</v>
       </c>
       <c r="I23" s="10">
-        <v>0.33249499999999999</v>
+        <v>0.368064</v>
       </c>
       <c r="J23" s="10">
-        <v>360.83532200000002</v>
+        <v>363.62221099999999</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1095,102 +1086,102 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="J27" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7">
         <f>AVERAGE(C14:C23)</f>
-        <v>0.99512</v>
+        <v>0.99497000000000002</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" ref="D28:J28" si="0">AVERAGE(D14:D23)</f>
-        <v>0.99512</v>
+        <v>0.99497000000000002</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>0.5482085000000001</v>
+        <v>0.5285398</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="0"/>
-        <v>0.99512</v>
+        <v>0.99497000000000002</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="0"/>
-        <v>0.36441829999999997</v>
+        <v>0.35498079999999999</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>0.99512</v>
+        <v>0.99497000000000002</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="0"/>
-        <v>0.3834283</v>
+        <v>0.36960989999999999</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>365.91393970000001</v>
+        <v>362.16446869999999</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3">
         <f>STDEV(C14:C23)</f>
-        <v>2.5328113497323398E-4</v>
+        <v>1.5767899881297446E-4</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" ref="D29:J29" si="1">STDEV(D14:D23)</f>
-        <v>2.5328113497323398E-4</v>
+        <v>1.5767899881297446E-4</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>0.12969930973709004</v>
+        <v>9.6161745462528245E-2</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>2.5328113497323398E-4</v>
+        <v>1.5767899881297446E-4</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>2.0609785054946862E-2</v>
+        <v>1.0965503148004145E-2</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
-        <v>2.5328113497323398E-4</v>
+        <v>1.5767899881297446E-4</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>3.1425952537671796E-2</v>
+        <v>1.7272011138447847E-2</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>8.4039577478257552</v>
+        <v>1.9219112871326809</v>
       </c>
     </row>
   </sheetData>
@@ -1203,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F4AF173-655A-42AC-ABF5-0B69C1546DB5}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,37 +1238,33 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1295,9 +1282,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1316,7 +1301,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -1329,7 +1314,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -1351,31 +1336,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1383,28 +1368,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="10">
-        <v>0.99539800000000001</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="D14" s="10">
-        <v>0.99539800000000001</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="E14" s="10">
-        <v>0.55887500000000001</v>
+        <v>0.60943499999999995</v>
       </c>
       <c r="F14" s="10">
-        <v>0.99539800000000001</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="G14" s="10">
-        <v>0.34120099999999998</v>
+        <v>0.35136099999999998</v>
       </c>
       <c r="H14" s="10">
-        <v>0.99539800000000001</v>
+        <v>0.99478100000000003</v>
       </c>
       <c r="I14" s="10">
-        <v>0.347412</v>
+        <v>0.36441200000000001</v>
       </c>
       <c r="J14" s="10">
-        <v>379.12150000000003</v>
+        <v>471.87817799999999</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1412,28 +1397,28 @@
         <v>2</v>
       </c>
       <c r="C15" s="10">
-        <v>0.995062</v>
+        <v>0.994973</v>
       </c>
       <c r="D15" s="10">
-        <v>0.995062</v>
+        <v>0.994973</v>
       </c>
       <c r="E15" s="10">
-        <v>0.62660000000000005</v>
+        <v>0.80349000000000004</v>
       </c>
       <c r="F15" s="10">
-        <v>0.995062</v>
+        <v>0.994973</v>
       </c>
       <c r="G15" s="10">
-        <v>0.36513200000000001</v>
+        <v>0.38317800000000002</v>
       </c>
       <c r="H15" s="10">
-        <v>0.995062</v>
+        <v>0.994973</v>
       </c>
       <c r="I15" s="10">
-        <v>0.38389299999999998</v>
+        <v>0.40745100000000001</v>
       </c>
       <c r="J15" s="10">
-        <v>364.07150100000001</v>
+        <v>474.32367900000003</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1441,28 +1426,28 @@
         <v>3</v>
       </c>
       <c r="C16" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99502000000000002</v>
       </c>
       <c r="D16" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99502000000000002</v>
       </c>
       <c r="E16" s="10">
-        <v>0.33167600000000003</v>
+        <v>0.65587799999999996</v>
       </c>
       <c r="F16" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99502000000000002</v>
       </c>
       <c r="G16" s="10">
-        <v>0.33333299999999999</v>
+        <v>0.34654499999999999</v>
       </c>
       <c r="H16" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99502000000000002</v>
       </c>
       <c r="I16" s="10">
-        <v>0.33250200000000002</v>
+        <v>0.35700599999999999</v>
       </c>
       <c r="J16" s="10">
-        <v>364.30012499999998</v>
+        <v>491.11946899999998</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -1470,28 +1455,28 @@
         <v>4</v>
       </c>
       <c r="C17" s="10">
-        <v>0.99510900000000002</v>
+        <v>0.99488299999999996</v>
       </c>
       <c r="D17" s="10">
-        <v>0.99510900000000002</v>
+        <v>0.99488299999999996</v>
       </c>
       <c r="E17" s="10">
-        <v>0.68362800000000001</v>
+        <v>0.52218399999999998</v>
       </c>
       <c r="F17" s="10">
-        <v>0.99510900000000002</v>
+        <v>0.99488299999999996</v>
       </c>
       <c r="G17" s="10">
-        <v>0.36145500000000003</v>
+        <v>0.352377</v>
       </c>
       <c r="H17" s="10">
-        <v>0.99510900000000002</v>
+        <v>0.99488299999999996</v>
       </c>
       <c r="I17" s="10">
-        <v>0.38427499999999998</v>
+        <v>0.36674099999999998</v>
       </c>
       <c r="J17" s="10">
-        <v>365.18265600000001</v>
+        <v>488.00500199999999</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1499,28 +1484,28 @@
         <v>5</v>
       </c>
       <c r="C18" s="10">
-        <v>0.99463699999999999</v>
+        <v>0.99522999999999995</v>
       </c>
       <c r="D18" s="10">
-        <v>0.99463699999999999</v>
+        <v>0.99522999999999995</v>
       </c>
       <c r="E18" s="10">
-        <v>0.57716699999999999</v>
+        <v>0.57756600000000002</v>
       </c>
       <c r="F18" s="10">
-        <v>0.99463699999999999</v>
+        <v>0.99522999999999995</v>
       </c>
       <c r="G18" s="10">
-        <v>0.35217700000000002</v>
+        <v>0.344999</v>
       </c>
       <c r="H18" s="10">
-        <v>0.99463699999999999</v>
+        <v>0.99522999999999995</v>
       </c>
       <c r="I18" s="10">
-        <v>0.36474099999999998</v>
+        <v>0.35311300000000001</v>
       </c>
       <c r="J18" s="10">
-        <v>363.32779499999998</v>
+        <v>489.83605699999998</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -1528,28 +1513,28 @@
         <v>6</v>
       </c>
       <c r="C19" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99509400000000003</v>
       </c>
       <c r="D19" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99509400000000003</v>
       </c>
       <c r="E19" s="10">
-        <v>0.59808399999999995</v>
+        <v>0.56504399999999999</v>
       </c>
       <c r="F19" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99509400000000003</v>
       </c>
       <c r="G19" s="10">
-        <v>0.36632399999999998</v>
+        <v>0.33651199999999998</v>
       </c>
       <c r="H19" s="10">
-        <v>0.99502699999999999</v>
+        <v>0.99509400000000003</v>
       </c>
       <c r="I19" s="10">
-        <v>0.391179</v>
+        <v>0.33879399999999998</v>
       </c>
       <c r="J19" s="10">
-        <v>384.73805299999998</v>
+        <v>487.36326100000002</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1557,28 +1542,28 @@
         <v>7</v>
       </c>
       <c r="C20" s="10">
-        <v>0.99504300000000001</v>
+        <v>0.99559399999999998</v>
       </c>
       <c r="D20" s="10">
-        <v>0.99504300000000001</v>
+        <v>0.99559399999999998</v>
       </c>
       <c r="E20" s="10">
-        <v>0.56552000000000002</v>
+        <v>0.44525100000000001</v>
       </c>
       <c r="F20" s="10">
-        <v>0.99504300000000001</v>
+        <v>0.99559399999999998</v>
       </c>
       <c r="G20" s="10">
-        <v>0.34657399999999999</v>
+        <v>0.35200599999999999</v>
       </c>
       <c r="H20" s="10">
-        <v>0.99504300000000001</v>
+        <v>0.99559399999999998</v>
       </c>
       <c r="I20" s="10">
-        <v>0.35714400000000002</v>
+        <v>0.36471500000000001</v>
       </c>
       <c r="J20" s="10">
-        <v>414.65117299999997</v>
+        <v>490.21203700000001</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1586,28 +1571,28 @@
         <v>8</v>
       </c>
       <c r="C21" s="10">
-        <v>0.99498799999999998</v>
+        <v>0.99503900000000001</v>
       </c>
       <c r="D21" s="10">
-        <v>0.99498799999999998</v>
+        <v>0.99503900000000001</v>
       </c>
       <c r="E21" s="10">
-        <v>0.55171000000000003</v>
+        <v>0.77338099999999999</v>
       </c>
       <c r="F21" s="10">
-        <v>0.99498799999999998</v>
+        <v>0.99503900000000001</v>
       </c>
       <c r="G21" s="10">
-        <v>0.35972500000000002</v>
+        <v>0.34653400000000001</v>
       </c>
       <c r="H21" s="10">
-        <v>0.99498799999999998</v>
+        <v>0.99503900000000001</v>
       </c>
       <c r="I21" s="10">
-        <v>0.37584200000000001</v>
+        <v>0.35664499999999999</v>
       </c>
       <c r="J21" s="10">
-        <v>417.22400199999998</v>
+        <v>487.64461599999998</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1615,28 +1600,28 @@
         <v>9</v>
       </c>
       <c r="C22" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99530099999999999</v>
       </c>
       <c r="D22" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99530099999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>0.58810499999999999</v>
+        <v>0.61031100000000005</v>
       </c>
       <c r="F22" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99530099999999999</v>
       </c>
       <c r="G22" s="10">
-        <v>0.36314800000000003</v>
+        <v>0.34895900000000002</v>
       </c>
       <c r="H22" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99530099999999999</v>
       </c>
       <c r="I22" s="10">
-        <v>0.38511600000000001</v>
+        <v>0.362153</v>
       </c>
       <c r="J22" s="10">
-        <v>394.02264700000001</v>
+        <v>488.87577800000003</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -1644,28 +1629,28 @@
         <v>10</v>
       </c>
       <c r="C23" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99539100000000003</v>
       </c>
       <c r="D23" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99539100000000003</v>
       </c>
       <c r="E23" s="10">
-        <v>0.58810499999999999</v>
+        <v>0.42515900000000001</v>
       </c>
       <c r="F23" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99539100000000003</v>
       </c>
       <c r="G23" s="10">
-        <v>0.36314800000000003</v>
+        <v>0.336063</v>
       </c>
       <c r="H23" s="10">
-        <v>0.99522999999999995</v>
+        <v>0.99539100000000003</v>
       </c>
       <c r="I23" s="10">
-        <v>0.38511600000000001</v>
+        <v>0.33789400000000003</v>
       </c>
       <c r="J23" s="10">
-        <v>394.02264700000001</v>
+        <v>487.35062099999999</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1704,102 +1689,102 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="J27" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7">
         <f>AVERAGE(C14:C23)</f>
-        <v>0.99507509999999999</v>
+        <v>0.99513059999999987</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" ref="D28:J28" si="0">AVERAGE(D14:D23)</f>
-        <v>0.99507509999999999</v>
+        <v>0.99513059999999987</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>0.56694699999999998</v>
+        <v>0.59876989999999997</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="0"/>
-        <v>0.99507509999999999</v>
+        <v>0.99513059999999987</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="0"/>
-        <v>0.35522169999999997</v>
+        <v>0.34985340000000004</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>0.99507509999999999</v>
+        <v>0.99513059999999987</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="0"/>
-        <v>0.370722</v>
+        <v>0.36089239999999995</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>384.06620989999993</v>
+        <v>485.6608698</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3">
         <f>STDEV(C14:C23)</f>
-        <v>1.9965216975752312E-4</v>
+        <v>2.4760865179642187E-4</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" ref="D29:J29" si="1">STDEV(D14:D23)</f>
-        <v>1.9965216975752312E-4</v>
+        <v>2.4760865179642187E-4</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>9.1161652750607031E-2</v>
+        <v>0.123409377935075</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>1.9965216975752312E-4</v>
+        <v>2.4760865179642187E-4</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>1.1382293481544055E-2</v>
+        <v>1.3073727813188305E-2</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
-        <v>1.9965216975752312E-4</v>
+        <v>2.4760865179642187E-4</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>1.9551912995351056E-2</v>
+        <v>1.9268360895519889E-2</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>20.642994265212497</v>
+        <v>6.7655609865150383</v>
       </c>
     </row>
   </sheetData>
@@ -1812,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72424044-ED58-4C86-AD31-3A2E055D2E2E}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1856,37 +1841,33 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1904,9 +1885,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1925,7 +1904,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -1938,7 +1917,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -1960,31 +1939,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1992,28 +1971,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="10">
-        <v>0.99184300000000003</v>
+        <v>0.99134</v>
       </c>
       <c r="D14" s="10">
-        <v>0.99184300000000003</v>
+        <v>0.99134</v>
       </c>
       <c r="E14" s="10">
-        <v>0.96406899999999995</v>
+        <v>0.96149700000000005</v>
       </c>
       <c r="F14" s="10">
-        <v>0.99184300000000003</v>
+        <v>0.99134</v>
       </c>
       <c r="G14" s="10">
-        <v>0.97158500000000003</v>
+        <v>0.95684199999999997</v>
       </c>
       <c r="H14" s="10">
-        <v>0.99184300000000003</v>
+        <v>0.99134</v>
       </c>
       <c r="I14" s="10">
-        <v>0.96760400000000002</v>
+        <v>0.95857300000000001</v>
       </c>
       <c r="J14" s="10">
-        <v>113.780996</v>
+        <v>103.77699800000001</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2021,28 +2000,28 @@
         <v>2</v>
       </c>
       <c r="C15" s="10">
-        <v>0.99226700000000001</v>
+        <v>0.98947300000000005</v>
       </c>
       <c r="D15" s="10">
-        <v>0.99226700000000001</v>
+        <v>0.98947300000000005</v>
       </c>
       <c r="E15" s="10">
-        <v>0.95689100000000005</v>
+        <v>0.95002299999999995</v>
       </c>
       <c r="F15" s="10">
-        <v>0.99226700000000001</v>
+        <v>0.98947300000000005</v>
       </c>
       <c r="G15" s="10">
-        <v>0.97728199999999998</v>
+        <v>0.95550199999999996</v>
       </c>
       <c r="H15" s="10">
-        <v>0.99226700000000001</v>
+        <v>0.98947300000000005</v>
       </c>
       <c r="I15" s="10">
-        <v>0.96677400000000002</v>
+        <v>0.95266899999999999</v>
       </c>
       <c r="J15" s="10">
-        <v>100.590002</v>
+        <v>100.01903</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2050,28 +2029,28 @@
         <v>3</v>
       </c>
       <c r="C16" s="10">
-        <v>0.98816199999999998</v>
+        <v>0.991228</v>
       </c>
       <c r="D16" s="10">
-        <v>0.98816199999999998</v>
+        <v>0.991228</v>
       </c>
       <c r="E16" s="10">
-        <v>0.95896899999999996</v>
+        <v>0.96220399999999995</v>
       </c>
       <c r="F16" s="10">
-        <v>0.98816199999999998</v>
+        <v>0.991228</v>
       </c>
       <c r="G16" s="10">
-        <v>0.91305599999999998</v>
+        <v>0.94879199999999997</v>
       </c>
       <c r="H16" s="10">
-        <v>0.98816199999999998</v>
+        <v>0.991228</v>
       </c>
       <c r="I16" s="10">
-        <v>0.93447599999999997</v>
+        <v>0.95499100000000003</v>
       </c>
       <c r="J16" s="10">
-        <v>100.867003</v>
+        <v>100.24597</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -2079,28 +2058,28 @@
         <v>4</v>
       </c>
       <c r="C17" s="10">
-        <v>0.98368299999999997</v>
+        <v>0.99122399999999999</v>
       </c>
       <c r="D17" s="10">
-        <v>0.98368299999999997</v>
+        <v>0.99122399999999999</v>
       </c>
       <c r="E17" s="10">
-        <v>0.89580700000000002</v>
+        <v>0.94816800000000001</v>
       </c>
       <c r="F17" s="10">
-        <v>0.98368299999999997</v>
+        <v>0.99122399999999999</v>
       </c>
       <c r="G17" s="10">
-        <v>0.96337399999999995</v>
+        <v>0.97208600000000001</v>
       </c>
       <c r="H17" s="10">
-        <v>0.98368299999999997</v>
+        <v>0.99122399999999999</v>
       </c>
       <c r="I17" s="10">
-        <v>0.927423</v>
+        <v>0.95981300000000003</v>
       </c>
       <c r="J17" s="10">
-        <v>100.97800100000001</v>
+        <v>100.06403</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -2108,28 +2087,28 @@
         <v>5</v>
       </c>
       <c r="C18" s="10">
-        <v>0.99056900000000003</v>
+        <v>0.98835499999999998</v>
       </c>
       <c r="D18" s="10">
-        <v>0.99056900000000003</v>
+        <v>0.98835499999999998</v>
       </c>
       <c r="E18" s="10">
-        <v>0.94324300000000005</v>
+        <v>0.92604399999999998</v>
       </c>
       <c r="F18" s="10">
-        <v>0.99056900000000003</v>
+        <v>0.98835499999999998</v>
       </c>
       <c r="G18" s="10">
-        <v>0.96636200000000005</v>
+        <v>0.966472</v>
       </c>
       <c r="H18" s="10">
-        <v>0.99056900000000003</v>
+        <v>0.98835499999999998</v>
       </c>
       <c r="I18" s="10">
-        <v>0.95456200000000002</v>
+        <v>0.94545900000000005</v>
       </c>
       <c r="J18" s="10">
-        <v>100.47502900000001</v>
+        <v>100.479028</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -2137,28 +2116,28 @@
         <v>6</v>
       </c>
       <c r="C19" s="10">
-        <v>0.98747200000000002</v>
+        <v>0.99238499999999996</v>
       </c>
       <c r="D19" s="10">
-        <v>0.98747200000000002</v>
+        <v>0.99238499999999996</v>
       </c>
       <c r="E19" s="10">
-        <v>0.93081499999999995</v>
+        <v>0.95342300000000002</v>
       </c>
       <c r="F19" s="10">
-        <v>0.98747200000000002</v>
+        <v>0.99238499999999996</v>
       </c>
       <c r="G19" s="10">
-        <v>0.95316400000000001</v>
+        <v>0.97456600000000004</v>
       </c>
       <c r="H19" s="10">
-        <v>0.98747200000000002</v>
+        <v>0.99238499999999996</v>
       </c>
       <c r="I19" s="10">
-        <v>0.94046700000000005</v>
+        <v>0.96378299999999995</v>
       </c>
       <c r="J19" s="10">
-        <v>101.199029</v>
+        <v>100.418999</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -2166,28 +2145,28 @@
         <v>7</v>
       </c>
       <c r="C20" s="10">
-        <v>0.990097</v>
+        <v>0.98835300000000004</v>
       </c>
       <c r="D20" s="10">
-        <v>0.990097</v>
+        <v>0.98835300000000004</v>
       </c>
       <c r="E20" s="10">
-        <v>0.93972500000000003</v>
+        <v>0.93452400000000002</v>
       </c>
       <c r="F20" s="10">
-        <v>0.990097</v>
+        <v>0.98835300000000004</v>
       </c>
       <c r="G20" s="10">
-        <v>0.96822699999999995</v>
+        <v>0.95405300000000004</v>
       </c>
       <c r="H20" s="10">
-        <v>0.990097</v>
+        <v>0.98835300000000004</v>
       </c>
       <c r="I20" s="10">
-        <v>0.95353699999999997</v>
+        <v>0.94288499999999997</v>
       </c>
       <c r="J20" s="10">
-        <v>100.505996</v>
+        <v>100.404004</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -2195,28 +2174,28 @@
         <v>8</v>
       </c>
       <c r="C21" s="10">
-        <v>0.98612999999999995</v>
+        <v>0.98916099999999996</v>
       </c>
       <c r="D21" s="10">
-        <v>0.98612999999999995</v>
+        <v>0.98916099999999996</v>
       </c>
       <c r="E21" s="10">
-        <v>0.91927899999999996</v>
+        <v>0.92922499999999997</v>
       </c>
       <c r="F21" s="10">
-        <v>0.98612999999999995</v>
+        <v>0.98916099999999996</v>
       </c>
       <c r="G21" s="10">
-        <v>0.97117100000000001</v>
+        <v>0.96866699999999994</v>
       </c>
       <c r="H21" s="10">
-        <v>0.98612999999999995</v>
+        <v>0.98916099999999996</v>
       </c>
       <c r="I21" s="10">
-        <v>0.94329399999999997</v>
+        <v>0.94818999999999998</v>
       </c>
       <c r="J21" s="10">
-        <v>100.92903</v>
+        <v>101.90499800000001</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -2224,28 +2203,28 @@
         <v>9</v>
       </c>
       <c r="C22" s="10">
-        <v>0.99008799999999997</v>
+        <v>0.99029599999999995</v>
       </c>
       <c r="D22" s="10">
-        <v>0.99008799999999997</v>
+        <v>0.99029599999999995</v>
       </c>
       <c r="E22" s="10">
-        <v>0.94402200000000003</v>
+        <v>0.93818999999999997</v>
       </c>
       <c r="F22" s="10">
-        <v>0.99008799999999997</v>
+        <v>0.99029599999999995</v>
       </c>
       <c r="G22" s="10">
-        <v>0.96234399999999998</v>
+        <v>0.97071799999999997</v>
       </c>
       <c r="H22" s="10">
-        <v>0.99008799999999997</v>
+        <v>0.99029599999999995</v>
       </c>
       <c r="I22" s="10">
-        <v>0.95302100000000001</v>
+        <v>0.95392500000000002</v>
       </c>
       <c r="J22" s="10">
-        <v>100.48299799999999</v>
+        <v>101.08699900000001</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -2253,28 +2232,28 @@
         <v>10</v>
       </c>
       <c r="C23" s="10">
-        <v>0.98824599999999996</v>
+        <v>0.98932900000000001</v>
       </c>
       <c r="D23" s="10">
-        <v>0.98824599999999996</v>
+        <v>0.98932900000000001</v>
       </c>
       <c r="E23" s="10">
-        <v>0.92048200000000002</v>
+        <v>0.94329799999999997</v>
       </c>
       <c r="F23" s="10">
-        <v>0.98824599999999996</v>
+        <v>0.98932900000000001</v>
       </c>
       <c r="G23" s="10">
-        <v>0.96475100000000003</v>
+        <v>0.95915300000000003</v>
       </c>
       <c r="H23" s="10">
-        <v>0.98824599999999996</v>
+        <v>0.98932900000000001</v>
       </c>
       <c r="I23" s="10">
-        <v>0.94152000000000002</v>
+        <v>0.95084299999999999</v>
       </c>
       <c r="J23" s="10">
-        <v>100.83002999999999</v>
+        <v>100.458001</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -2313,102 +2292,102 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="J27" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7">
         <f>AVERAGE(C14:C23)</f>
-        <v>0.9888557</v>
+        <v>0.99011440000000006</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" ref="D28:J28" si="0">AVERAGE(D14:D23)</f>
-        <v>0.9888557</v>
+        <v>0.99011440000000006</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>0.93733020000000011</v>
+        <v>0.94465959999999993</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="0"/>
-        <v>0.9888557</v>
+        <v>0.99011440000000006</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="0"/>
-        <v>0.96113160000000009</v>
+        <v>0.96268510000000018</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>0.9888557</v>
+        <v>0.99011440000000006</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="0"/>
-        <v>0.94826779999999999</v>
+        <v>0.95311310000000016</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>102.06381139999999</v>
+        <v>100.88580569999999</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3">
         <f>STDEV(C14:C23)</f>
-        <v>2.6564295189010728E-3</v>
+        <v>1.3863321872240079E-3</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" ref="D29:J29" si="1">STDEV(D14:D23)</f>
-        <v>2.6564295189010728E-3</v>
+        <v>1.3863321872240079E-3</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>2.1154547920797864E-2</v>
+        <v>1.2650795435685286E-2</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>2.6564295189010728E-3</v>
+        <v>1.3863321872240079E-3</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>1.8082971186542701E-2</v>
+        <v>8.88150249363499E-3</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
-        <v>2.6564295189010728E-3</v>
+        <v>1.3863321872240079E-3</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>1.3174832099288577E-2</v>
+        <v>6.5448741003084881E-3</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>4.1242325478382096</v>
+        <v>1.1581957267897411</v>
       </c>
     </row>
   </sheetData>
@@ -2422,7 +2401,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2457,7 +2436,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2465,37 +2444,33 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2513,9 +2488,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2534,7 +2507,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -2547,7 +2520,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -2569,31 +2542,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2601,28 +2574,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="10">
-        <v>0.96897299999999997</v>
+        <v>0.96512799999999999</v>
       </c>
       <c r="D14" s="10">
-        <v>0.96897299999999997</v>
+        <v>0.96512799999999999</v>
       </c>
       <c r="E14" s="10">
-        <v>0.82403000000000004</v>
+        <v>0.82728000000000002</v>
       </c>
       <c r="F14" s="10">
-        <v>0.96897299999999997</v>
+        <v>0.96512799999999999</v>
       </c>
       <c r="G14" s="10">
-        <v>0.82607600000000003</v>
+        <v>0.81651499999999999</v>
       </c>
       <c r="H14" s="10">
-        <v>0.96897299999999997</v>
+        <v>0.96512799999999999</v>
       </c>
       <c r="I14" s="10">
-        <v>0.82347800000000004</v>
+        <v>0.816191</v>
       </c>
       <c r="J14" s="10">
-        <v>114.479259</v>
+        <v>104.859754</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2630,28 +2603,28 @@
         <v>2</v>
       </c>
       <c r="C15" s="10">
-        <v>0.96337099999999998</v>
+        <v>0.96736699999999998</v>
       </c>
       <c r="D15" s="10">
-        <v>0.96337099999999998</v>
+        <v>0.96736699999999998</v>
       </c>
       <c r="E15" s="10">
-        <v>0.83896999999999999</v>
+        <v>0.86112900000000003</v>
       </c>
       <c r="F15" s="10">
-        <v>0.96337099999999998</v>
+        <v>0.96736699999999998</v>
       </c>
       <c r="G15" s="10">
-        <v>0.80114600000000002</v>
+        <v>0.77149800000000002</v>
       </c>
       <c r="H15" s="10">
-        <v>0.96337099999999998</v>
+        <v>0.96736699999999998</v>
       </c>
       <c r="I15" s="10">
-        <v>0.79874199999999995</v>
+        <v>0.80293300000000001</v>
       </c>
       <c r="J15" s="10">
-        <v>110.475375</v>
+        <v>102.99825800000001</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2659,28 +2632,28 @@
         <v>3</v>
       </c>
       <c r="C16" s="10">
-        <v>0.97080999999999995</v>
+        <v>0.96926199999999996</v>
       </c>
       <c r="D16" s="10">
-        <v>0.97080999999999995</v>
+        <v>0.96926199999999996</v>
       </c>
       <c r="E16" s="10">
-        <v>0.84872300000000001</v>
+        <v>0.83399100000000004</v>
       </c>
       <c r="F16" s="10">
-        <v>0.97080999999999995</v>
+        <v>0.96926199999999996</v>
       </c>
       <c r="G16" s="10">
-        <v>0.82629900000000001</v>
+        <v>0.84688200000000002</v>
       </c>
       <c r="H16" s="10">
-        <v>0.97080999999999995</v>
+        <v>0.96926199999999996</v>
       </c>
       <c r="I16" s="10">
-        <v>0.83626400000000001</v>
+        <v>0.83995900000000001</v>
       </c>
       <c r="J16" s="10">
-        <v>107.79512699999999</v>
+        <v>101.319661</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -2688,28 +2661,28 @@
         <v>4</v>
       </c>
       <c r="C17" s="10">
-        <v>0.96662000000000003</v>
+        <v>0.96520300000000003</v>
       </c>
       <c r="D17" s="10">
-        <v>0.96662000000000003</v>
+        <v>0.96520300000000003</v>
       </c>
       <c r="E17" s="10">
-        <v>0.80369000000000002</v>
+        <v>0.82256700000000005</v>
       </c>
       <c r="F17" s="10">
-        <v>0.96662000000000003</v>
+        <v>0.96520300000000003</v>
       </c>
       <c r="G17" s="10">
-        <v>0.84374300000000002</v>
+        <v>0.86972499999999997</v>
       </c>
       <c r="H17" s="10">
-        <v>0.96662000000000003</v>
+        <v>0.96520300000000003</v>
       </c>
       <c r="I17" s="10">
-        <v>0.82187100000000002</v>
+        <v>0.84465400000000002</v>
       </c>
       <c r="J17" s="10">
-        <v>113.568082</v>
+        <v>101.06237900000001</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -2717,28 +2690,28 @@
         <v>5</v>
       </c>
       <c r="C18" s="10">
-        <v>0.96796599999999999</v>
+        <v>0.96778600000000004</v>
       </c>
       <c r="D18" s="10">
-        <v>0.96796599999999999</v>
+        <v>0.96778600000000004</v>
       </c>
       <c r="E18" s="10">
-        <v>0.82764800000000005</v>
+        <v>0.84873200000000004</v>
       </c>
       <c r="F18" s="10">
-        <v>0.96796599999999999</v>
+        <v>0.96778600000000004</v>
       </c>
       <c r="G18" s="10">
-        <v>0.83243400000000001</v>
+        <v>0.81588799999999995</v>
       </c>
       <c r="H18" s="10">
-        <v>0.96796599999999999</v>
+        <v>0.96778600000000004</v>
       </c>
       <c r="I18" s="10">
-        <v>0.82748299999999997</v>
+        <v>0.82750500000000005</v>
       </c>
       <c r="J18" s="10">
-        <v>113.804849</v>
+        <v>100.821145</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -2746,28 +2719,28 @@
         <v>6</v>
       </c>
       <c r="C19" s="10">
-        <v>0.97073699999999996</v>
+        <v>0.96146399999999999</v>
       </c>
       <c r="D19" s="10">
-        <v>0.97073699999999996</v>
+        <v>0.96146399999999999</v>
       </c>
       <c r="E19" s="10">
-        <v>0.84915700000000005</v>
+        <v>0.76075400000000004</v>
       </c>
       <c r="F19" s="10">
-        <v>0.97073699999999996</v>
+        <v>0.96146399999999999</v>
       </c>
       <c r="G19" s="10">
-        <v>0.84281899999999998</v>
+        <v>0.83170299999999997</v>
       </c>
       <c r="H19" s="10">
-        <v>0.97073699999999996</v>
+        <v>0.96146399999999999</v>
       </c>
       <c r="I19" s="10">
-        <v>0.84471099999999999</v>
+        <v>0.79307499999999997</v>
       </c>
       <c r="J19" s="10">
-        <v>108.59209199999999</v>
+        <v>100.97201699999999</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -2775,28 +2748,28 @@
         <v>7</v>
       </c>
       <c r="C20" s="10">
-        <v>0.95405399999999996</v>
+        <v>0.971329</v>
       </c>
       <c r="D20" s="10">
-        <v>0.95405399999999996</v>
+        <v>0.971329</v>
       </c>
       <c r="E20" s="10">
-        <v>0.75621700000000003</v>
+        <v>0.83579499999999995</v>
       </c>
       <c r="F20" s="10">
-        <v>0.95405399999999996</v>
+        <v>0.971329</v>
       </c>
       <c r="G20" s="10">
-        <v>0.66843600000000003</v>
+        <v>0.83129600000000003</v>
       </c>
       <c r="H20" s="10">
-        <v>0.95405399999999996</v>
+        <v>0.971329</v>
       </c>
       <c r="I20" s="10">
-        <v>0.63983599999999996</v>
+        <v>0.83175100000000002</v>
       </c>
       <c r="J20" s="10">
-        <v>111.354443</v>
+        <v>101.05466</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -2804,28 +2777,28 @@
         <v>8</v>
       </c>
       <c r="C21" s="10">
-        <v>0.97152799999999995</v>
+        <v>0.96458600000000005</v>
       </c>
       <c r="D21" s="10">
-        <v>0.97152799999999995</v>
+        <v>0.96458600000000005</v>
       </c>
       <c r="E21" s="10">
-        <v>0.85004000000000002</v>
+        <v>0.78420599999999996</v>
       </c>
       <c r="F21" s="10">
-        <v>0.97152799999999995</v>
+        <v>0.96458600000000005</v>
       </c>
       <c r="G21" s="10">
-        <v>0.85055700000000001</v>
+        <v>0.86723799999999995</v>
       </c>
       <c r="H21" s="10">
-        <v>0.97152799999999995</v>
+        <v>0.96458600000000005</v>
       </c>
       <c r="I21" s="10">
-        <v>0.85029699999999997</v>
+        <v>0.82163200000000003</v>
       </c>
       <c r="J21" s="10">
-        <v>111.676461</v>
+        <v>101.390086</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -2833,28 +2806,28 @@
         <v>9</v>
       </c>
       <c r="C22" s="10">
-        <v>0.96430499999999997</v>
+        <v>0.96399699999999999</v>
       </c>
       <c r="D22" s="10">
-        <v>0.96430499999999997</v>
+        <v>0.96399699999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>0.80072600000000005</v>
+        <v>0.82638400000000001</v>
       </c>
       <c r="F22" s="10">
-        <v>0.96430499999999997</v>
+        <v>0.96399699999999999</v>
       </c>
       <c r="G22" s="10">
-        <v>0.86585699999999999</v>
+        <v>0.83800699999999995</v>
       </c>
       <c r="H22" s="10">
-        <v>0.96430499999999997</v>
+        <v>0.96399699999999999</v>
       </c>
       <c r="I22" s="10">
-        <v>0.81686400000000003</v>
+        <v>0.82524200000000003</v>
       </c>
       <c r="J22" s="10">
-        <v>110.984551</v>
+        <v>101.483335</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -2862,28 +2835,28 @@
         <v>10</v>
       </c>
       <c r="C23" s="10">
-        <v>0.96912200000000004</v>
+        <v>0.96740400000000004</v>
       </c>
       <c r="D23" s="10">
-        <v>0.96912200000000004</v>
+        <v>0.96740400000000004</v>
       </c>
       <c r="E23" s="10">
-        <v>0.82139799999999996</v>
+        <v>0.83969099999999997</v>
       </c>
       <c r="F23" s="10">
-        <v>0.96912200000000004</v>
+        <v>0.96740400000000004</v>
       </c>
       <c r="G23" s="10">
-        <v>0.808392</v>
+        <v>0.79840199999999995</v>
       </c>
       <c r="H23" s="10">
-        <v>0.96912200000000004</v>
+        <v>0.96740400000000004</v>
       </c>
       <c r="I23" s="10">
-        <v>0.80640000000000001</v>
+        <v>0.80662999999999996</v>
       </c>
       <c r="J23" s="10">
-        <v>109.699027</v>
+        <v>100.968574</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -2922,102 +2895,102 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="J27" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7">
         <f>AVERAGE(C14:C23)</f>
-        <v>0.96674860000000007</v>
+        <v>0.96635259999999989</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" ref="D28:J28" si="0">AVERAGE(D14:D23)</f>
-        <v>0.96674860000000007</v>
+        <v>0.96635259999999989</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>0.82205989999999995</v>
+        <v>0.82405290000000009</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="0"/>
-        <v>0.96674860000000007</v>
+        <v>0.96635259999999989</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="0"/>
-        <v>0.81657589999999991</v>
+        <v>0.8287154000000001</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>0.96674860000000007</v>
+        <v>0.96635259999999989</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="0"/>
-        <v>0.80659460000000005</v>
+        <v>0.82095719999999994</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>111.2429266</v>
+        <v>101.69298690000001</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3">
         <f>STDEV(C14:C23)</f>
-        <v>5.2266069766999804E-3</v>
+        <v>2.8442458949800892E-3</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" ref="D29:J29" si="1">STDEV(D14:D23)</f>
-        <v>5.2266069766999804E-3</v>
+        <v>2.8442458949800892E-3</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>2.9206988263655892E-2</v>
+        <v>2.9958249401644137E-2</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>5.2266069766999804E-3</v>
+        <v>2.8442458949800892E-3</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>5.5474570259113606E-2</v>
+        <v>3.0007124103008157E-2</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
-        <v>5.2266069766999804E-3</v>
+        <v>2.8442458949800892E-3</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>6.071185890417128E-2</v>
+        <v>1.6435312888209149E-2</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>2.2260526834897818</v>
+        <v>1.2744074488838981</v>
       </c>
     </row>
   </sheetData>
@@ -3030,8 +3003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59A332C-4FAC-4179-A863-F1D9801446E1}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3066,7 +3039,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3074,37 +3047,33 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3122,9 +3091,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3143,7 +3110,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -3156,7 +3123,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -3178,31 +3145,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3210,28 +3177,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="10">
-        <v>0.99115699999999995</v>
+        <v>0.992788</v>
       </c>
       <c r="D14" s="10">
-        <v>0.99115699999999995</v>
+        <v>0.992788</v>
       </c>
       <c r="E14" s="10">
-        <v>0.94628999999999996</v>
+        <v>0.97055199999999997</v>
       </c>
       <c r="F14" s="10">
-        <v>0.99115699999999995</v>
+        <v>0.992788</v>
       </c>
       <c r="G14" s="10">
-        <v>0.97133499999999995</v>
+        <v>0.96506000000000003</v>
       </c>
       <c r="H14" s="10">
-        <v>0.99115699999999995</v>
+        <v>0.992788</v>
       </c>
       <c r="I14" s="10">
-        <v>0.95844300000000004</v>
+        <v>0.96779000000000004</v>
       </c>
       <c r="J14" s="10">
-        <v>105.077601</v>
+        <v>96.355030999999997</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3239,28 +3206,28 @@
         <v>2</v>
       </c>
       <c r="C15" s="10">
-        <v>0.99034599999999995</v>
+        <v>0.99222399999999999</v>
       </c>
       <c r="D15" s="10">
-        <v>0.99034599999999995</v>
+        <v>0.99222399999999999</v>
       </c>
       <c r="E15" s="10">
-        <v>0.93564499999999995</v>
+        <v>0.950183</v>
       </c>
       <c r="F15" s="10">
-        <v>0.99034599999999995</v>
+        <v>0.99222399999999999</v>
       </c>
       <c r="G15" s="10">
-        <v>0.97850899999999996</v>
+        <v>0.985151</v>
       </c>
       <c r="H15" s="10">
-        <v>0.99034599999999995</v>
+        <v>0.99222399999999999</v>
       </c>
       <c r="I15" s="10">
-        <v>0.95619799999999999</v>
+        <v>0.96711100000000005</v>
       </c>
       <c r="J15" s="10">
-        <v>95.691000000000003</v>
+        <v>93.304001</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3268,28 +3235,28 @@
         <v>3</v>
       </c>
       <c r="C16" s="10">
-        <v>0.99472000000000005</v>
+        <v>0.99404099999999995</v>
       </c>
       <c r="D16" s="10">
-        <v>0.99472000000000005</v>
+        <v>0.99404099999999995</v>
       </c>
       <c r="E16" s="10">
-        <v>0.97873500000000002</v>
+        <v>0.97090399999999999</v>
       </c>
       <c r="F16" s="10">
-        <v>0.99472000000000005</v>
+        <v>0.99404099999999995</v>
       </c>
       <c r="G16" s="10">
-        <v>0.98149500000000001</v>
+        <v>0.97516999999999998</v>
       </c>
       <c r="H16" s="10">
-        <v>0.99472000000000005</v>
+        <v>0.99404099999999995</v>
       </c>
       <c r="I16" s="10">
-        <v>0.98009199999999996</v>
+        <v>0.97302</v>
       </c>
       <c r="J16" s="10">
-        <v>95.344026999999997</v>
+        <v>94.293000000000006</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -3297,28 +3264,28 @@
         <v>4</v>
       </c>
       <c r="C17" s="10">
-        <v>0.99227699999999996</v>
+        <v>0.99176500000000001</v>
       </c>
       <c r="D17" s="10">
-        <v>0.99227699999999996</v>
+        <v>0.99176500000000001</v>
       </c>
       <c r="E17" s="10">
-        <v>0.95782500000000004</v>
+        <v>0.96666200000000002</v>
       </c>
       <c r="F17" s="10">
-        <v>0.99227699999999996</v>
+        <v>0.99176500000000001</v>
       </c>
       <c r="G17" s="10">
-        <v>0.97902100000000003</v>
+        <v>0.95382100000000003</v>
       </c>
       <c r="H17" s="10">
-        <v>0.99227699999999996</v>
+        <v>0.99176500000000001</v>
       </c>
       <c r="I17" s="10">
-        <v>0.96821599999999997</v>
+        <v>0.96012600000000003</v>
       </c>
       <c r="J17" s="10">
-        <v>95.486997000000002</v>
+        <v>93.671970000000002</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -3326,28 +3293,28 @@
         <v>5</v>
       </c>
       <c r="C18" s="10">
-        <v>0.99127799999999999</v>
+        <v>0.98825399999999997</v>
       </c>
       <c r="D18" s="10">
-        <v>0.99127799999999999</v>
+        <v>0.98825399999999997</v>
       </c>
       <c r="E18" s="10">
-        <v>0.946407</v>
+        <v>0.93581599999999998</v>
       </c>
       <c r="F18" s="10">
-        <v>0.99127799999999999</v>
+        <v>0.98825399999999997</v>
       </c>
       <c r="G18" s="10">
-        <v>0.96448400000000001</v>
+        <v>0.96527399999999997</v>
       </c>
       <c r="H18" s="10">
-        <v>0.99127799999999999</v>
+        <v>0.98825399999999997</v>
       </c>
       <c r="I18" s="10">
-        <v>0.95528599999999997</v>
+        <v>0.95003199999999999</v>
       </c>
       <c r="J18" s="10">
-        <v>96.287031999999996</v>
+        <v>93.385000000000005</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -3355,28 +3322,28 @@
         <v>6</v>
       </c>
       <c r="C19" s="10">
-        <v>0.98974399999999996</v>
+        <v>0.99099199999999998</v>
       </c>
       <c r="D19" s="10">
-        <v>0.98974399999999996</v>
+        <v>0.99099199999999998</v>
       </c>
       <c r="E19" s="10">
-        <v>0.95135000000000003</v>
+        <v>0.95180699999999996</v>
       </c>
       <c r="F19" s="10">
-        <v>0.98974399999999996</v>
+        <v>0.99099199999999998</v>
       </c>
       <c r="G19" s="10">
-        <v>0.95526500000000003</v>
+        <v>0.96142899999999998</v>
       </c>
       <c r="H19" s="10">
-        <v>0.98974399999999996</v>
+        <v>0.99099199999999998</v>
       </c>
       <c r="I19" s="10">
-        <v>0.95323500000000005</v>
+        <v>0.95657300000000001</v>
       </c>
       <c r="J19" s="10">
-        <v>95.160028999999994</v>
+        <v>95.040031999999997</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -3384,28 +3351,28 @@
         <v>7</v>
       </c>
       <c r="C20" s="10">
-        <v>0.98450099999999996</v>
+        <v>0.99141699999999999</v>
       </c>
       <c r="D20" s="10">
-        <v>0.98450099999999996</v>
+        <v>0.99141699999999999</v>
       </c>
       <c r="E20" s="10">
-        <v>0.91449400000000003</v>
+        <v>0.95775399999999999</v>
       </c>
       <c r="F20" s="10">
-        <v>0.98450099999999996</v>
+        <v>0.99141699999999999</v>
       </c>
       <c r="G20" s="10">
-        <v>0.96684199999999998</v>
+        <v>0.97266799999999998</v>
       </c>
       <c r="H20" s="10">
-        <v>0.98450099999999996</v>
+        <v>0.99141699999999999</v>
       </c>
       <c r="I20" s="10">
-        <v>0.93932199999999999</v>
+        <v>0.96498300000000004</v>
       </c>
       <c r="J20" s="10">
-        <v>95.744032000000004</v>
+        <v>93.354969999999994</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -3413,28 +3380,28 @@
         <v>8</v>
       </c>
       <c r="C21" s="10">
-        <v>0.99177499999999996</v>
+        <v>0.99189700000000003</v>
       </c>
       <c r="D21" s="10">
-        <v>0.99177499999999996</v>
+        <v>0.99189700000000003</v>
       </c>
       <c r="E21" s="10">
-        <v>0.95556200000000002</v>
+        <v>0.972993</v>
       </c>
       <c r="F21" s="10">
-        <v>0.99177499999999996</v>
+        <v>0.99189700000000003</v>
       </c>
       <c r="G21" s="10">
-        <v>0.96275200000000005</v>
+        <v>0.94765299999999997</v>
       </c>
       <c r="H21" s="10">
-        <v>0.99177499999999996</v>
+        <v>0.99189700000000003</v>
       </c>
       <c r="I21" s="10">
-        <v>0.95906100000000005</v>
+        <v>0.95967199999999997</v>
       </c>
       <c r="J21" s="10">
-        <v>95.143996999999999</v>
+        <v>93.714029999999994</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -3442,28 +3409,28 @@
         <v>9</v>
       </c>
       <c r="C22" s="10">
-        <v>0.98973500000000003</v>
+        <v>0.99016499999999996</v>
       </c>
       <c r="D22" s="10">
-        <v>0.98973500000000003</v>
+        <v>0.99016499999999996</v>
       </c>
       <c r="E22" s="10">
-        <v>0.93598400000000004</v>
+        <v>0.93181199999999997</v>
       </c>
       <c r="F22" s="10">
-        <v>0.98973500000000003</v>
+        <v>0.99016499999999996</v>
       </c>
       <c r="G22" s="10">
-        <v>0.96418199999999998</v>
+        <v>0.97670999999999997</v>
       </c>
       <c r="H22" s="10">
-        <v>0.98973500000000003</v>
+        <v>0.99016499999999996</v>
       </c>
       <c r="I22" s="10">
-        <v>0.949658</v>
+        <v>0.95333299999999999</v>
       </c>
       <c r="J22" s="10">
-        <v>96.333027999999999</v>
+        <v>94.031001000000003</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -3471,28 +3438,28 @@
         <v>10</v>
       </c>
       <c r="C23" s="10">
-        <v>0.99328899999999998</v>
+        <v>0.99116300000000002</v>
       </c>
       <c r="D23" s="10">
-        <v>0.99328899999999998</v>
+        <v>0.99116300000000002</v>
       </c>
       <c r="E23" s="10">
-        <v>0.96300600000000003</v>
+        <v>0.95562499999999995</v>
       </c>
       <c r="F23" s="10">
-        <v>0.99328899999999998</v>
+        <v>0.99116300000000002</v>
       </c>
       <c r="G23" s="10">
-        <v>0.97981499999999999</v>
+        <v>0.96976499999999999</v>
       </c>
       <c r="H23" s="10">
-        <v>0.99328899999999998</v>
+        <v>0.99116300000000002</v>
       </c>
       <c r="I23" s="10">
-        <v>0.97128000000000003</v>
+        <v>0.96228000000000002</v>
       </c>
       <c r="J23" s="10">
-        <v>97.102969000000002</v>
+        <v>94.227998999999997</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -3531,102 +3498,102 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="J27" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7">
         <f>AVERAGE(C14:C23)</f>
-        <v>0.99088220000000005</v>
+        <v>0.99147060000000009</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" ref="D28:J28" si="0">AVERAGE(D14:D23)</f>
-        <v>0.99088220000000005</v>
+        <v>0.99147060000000009</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>0.94852979999999998</v>
+        <v>0.95641079999999989</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="0"/>
-        <v>0.99088220000000005</v>
+        <v>0.99147060000000009</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="0"/>
-        <v>0.97036999999999995</v>
+        <v>0.96727010000000002</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>0.99088220000000005</v>
+        <v>0.99147060000000009</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="0"/>
-        <v>0.95907909999999996</v>
+        <v>0.96149200000000001</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>96.737071200000003</v>
+        <v>94.137703399999992</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3">
         <f>STDEV(C14:C23)</f>
-        <v>2.7307898246966464E-3</v>
+        <v>1.5476237843150998E-3</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" ref="D29:J29" si="1">STDEV(D14:D23)</f>
-        <v>2.7307898246966464E-3</v>
+        <v>1.5476237843150998E-3</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>1.7502680479159635E-2</v>
+        <v>1.4459643939061729E-2</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>2.7307898246966464E-3</v>
+        <v>1.5476237843150998E-3</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>8.9849631792975736E-3</v>
+        <v>1.113206019117755E-2</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
-        <v>2.7307898246966464E-3</v>
+        <v>1.5476237843150998E-3</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>1.1596138221647559E-2</v>
+        <v>7.0254819684409612E-3</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>2.9939327851485773</v>
+        <v>0.94546254082752679</v>
       </c>
     </row>
   </sheetData>
@@ -3639,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE8AD3C-79CA-4128-8DC0-6B0CEBFAB347}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J3"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3675,7 +3642,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3683,37 +3650,33 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3731,9 +3694,7 @@
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -3752,7 +3713,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>4</v>
@@ -3765,7 +3726,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>4</v>
@@ -3787,31 +3748,31 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="H13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="I13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3819,28 +3780,28 @@
         <v>1</v>
       </c>
       <c r="C14" s="10">
-        <v>0.98009299999999999</v>
+        <v>0.97384199999999999</v>
       </c>
       <c r="D14" s="10">
-        <v>0.98009299999999999</v>
+        <v>0.97384199999999999</v>
       </c>
       <c r="E14" s="10">
-        <v>0.90578999999999998</v>
+        <v>0.84177100000000005</v>
       </c>
       <c r="F14" s="10">
-        <v>0.98009299999999999</v>
+        <v>0.97384199999999999</v>
       </c>
       <c r="G14" s="10">
-        <v>0.90927100000000005</v>
+        <v>0.94140699999999999</v>
       </c>
       <c r="H14" s="10">
-        <v>0.98009299999999999</v>
+        <v>0.97384199999999999</v>
       </c>
       <c r="I14" s="10">
-        <v>0.90745699999999996</v>
+        <v>0.88618699999999995</v>
       </c>
       <c r="J14" s="10">
-        <v>99.004893999999993</v>
+        <v>95.567651999999995</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3848,28 +3809,28 @@
         <v>2</v>
       </c>
       <c r="C15" s="10">
-        <v>0.98114599999999996</v>
+        <v>0.97968699999999997</v>
       </c>
       <c r="D15" s="10">
-        <v>0.98114599999999996</v>
+        <v>0.97968699999999997</v>
       </c>
       <c r="E15" s="10">
-        <v>0.90873499999999996</v>
+        <v>0.91629400000000005</v>
       </c>
       <c r="F15" s="10">
-        <v>0.98114599999999996</v>
+        <v>0.97968699999999997</v>
       </c>
       <c r="G15" s="10">
-        <v>0.91803000000000001</v>
+        <v>0.90105800000000003</v>
       </c>
       <c r="H15" s="10">
-        <v>0.98114599999999996</v>
+        <v>0.97968699999999997</v>
       </c>
       <c r="I15" s="10">
-        <v>0.91313299999999997</v>
+        <v>0.90839499999999995</v>
       </c>
       <c r="J15" s="10">
-        <v>95.168508000000003</v>
+        <v>91.334953999999996</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3877,28 +3838,28 @@
         <v>3</v>
       </c>
       <c r="C16" s="10">
-        <v>0.97325499999999998</v>
+        <v>0.97603200000000001</v>
       </c>
       <c r="D16" s="10">
-        <v>0.97325499999999998</v>
+        <v>0.97603200000000001</v>
       </c>
       <c r="E16" s="10">
-        <v>0.86094800000000005</v>
+        <v>0.85933099999999996</v>
       </c>
       <c r="F16" s="10">
-        <v>0.97325499999999998</v>
+        <v>0.97603200000000001</v>
       </c>
       <c r="G16" s="10">
-        <v>0.89962299999999995</v>
+        <v>0.92553799999999997</v>
       </c>
       <c r="H16" s="10">
-        <v>0.97325499999999998</v>
+        <v>0.97603200000000001</v>
       </c>
       <c r="I16" s="10">
-        <v>0.879436</v>
+        <v>0.89017299999999999</v>
       </c>
       <c r="J16" s="10">
-        <v>94.875341000000006</v>
+        <v>95.048315000000002</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -3906,28 +3867,28 @@
         <v>4</v>
       </c>
       <c r="C17" s="10">
-        <v>0.981769</v>
+        <v>0.97975900000000005</v>
       </c>
       <c r="D17" s="10">
-        <v>0.981769</v>
+        <v>0.97975900000000005</v>
       </c>
       <c r="E17" s="10">
-        <v>0.92438600000000004</v>
+        <v>0.90393699999999999</v>
       </c>
       <c r="F17" s="10">
-        <v>0.981769</v>
+        <v>0.97975900000000005</v>
       </c>
       <c r="G17" s="10">
-        <v>0.896316</v>
+        <v>0.91415100000000005</v>
       </c>
       <c r="H17" s="10">
-        <v>0.981769</v>
+        <v>0.97975900000000005</v>
       </c>
       <c r="I17" s="10">
-        <v>0.908466</v>
+        <v>0.90728500000000001</v>
       </c>
       <c r="J17" s="10">
-        <v>95.501744000000002</v>
+        <v>95.601371999999998</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -3935,28 +3896,28 @@
         <v>5</v>
       </c>
       <c r="C18" s="10">
-        <v>0.97701499999999997</v>
+        <v>0.97824199999999994</v>
       </c>
       <c r="D18" s="10">
-        <v>0.97701499999999997</v>
+        <v>0.97824199999999994</v>
       </c>
       <c r="E18" s="10">
-        <v>0.880359</v>
+        <v>0.90203800000000001</v>
       </c>
       <c r="F18" s="10">
-        <v>0.97701499999999997</v>
+        <v>0.97824199999999994</v>
       </c>
       <c r="G18" s="10">
-        <v>0.90662699999999996</v>
+        <v>0.91556000000000004</v>
       </c>
       <c r="H18" s="10">
-        <v>0.97701499999999997</v>
+        <v>0.97824199999999994</v>
       </c>
       <c r="I18" s="10">
-        <v>0.892258</v>
+        <v>0.90556499999999995</v>
       </c>
       <c r="J18" s="10">
-        <v>96.837001000000001</v>
+        <v>96.182761999999997</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -3964,28 +3925,28 @@
         <v>6</v>
       </c>
       <c r="C19" s="10">
-        <v>0.98133899999999996</v>
+        <v>0.97284499999999996</v>
       </c>
       <c r="D19" s="10">
-        <v>0.98133899999999996</v>
+        <v>0.97284499999999996</v>
       </c>
       <c r="E19" s="10">
-        <v>0.91647699999999999</v>
+        <v>0.86792599999999998</v>
       </c>
       <c r="F19" s="10">
-        <v>0.98133899999999996</v>
+        <v>0.97284499999999996</v>
       </c>
       <c r="G19" s="10">
-        <v>0.90145399999999998</v>
+        <v>0.88833099999999998</v>
       </c>
       <c r="H19" s="10">
-        <v>0.98133899999999996</v>
+        <v>0.97284499999999996</v>
       </c>
       <c r="I19" s="10">
-        <v>0.90744499999999995</v>
+        <v>0.87787499999999996</v>
       </c>
       <c r="J19" s="10">
-        <v>92.344031999999999</v>
+        <v>96.182066000000006</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -3993,28 +3954,28 @@
         <v>7</v>
       </c>
       <c r="C20" s="10">
-        <v>0.97878500000000002</v>
+        <v>0.97809800000000002</v>
       </c>
       <c r="D20" s="10">
-        <v>0.97878500000000002</v>
+        <v>0.97809800000000002</v>
       </c>
       <c r="E20" s="10">
-        <v>0.87187899999999996</v>
+        <v>0.86893200000000004</v>
       </c>
       <c r="F20" s="10">
-        <v>0.97878500000000002</v>
+        <v>0.97809800000000002</v>
       </c>
       <c r="G20" s="10">
-        <v>0.93092799999999998</v>
+        <v>0.93646099999999999</v>
       </c>
       <c r="H20" s="10">
-        <v>0.97878500000000002</v>
+        <v>0.97809800000000002</v>
       </c>
       <c r="I20" s="10">
-        <v>0.89914400000000005</v>
+        <v>0.90038600000000002</v>
       </c>
       <c r="J20" s="10">
-        <v>91.709093999999993</v>
+        <v>96.276967999999997</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -4022,28 +3983,28 @@
         <v>8</v>
       </c>
       <c r="C21" s="10">
-        <v>0.97600399999999998</v>
+        <v>0.97783399999999998</v>
       </c>
       <c r="D21" s="10">
-        <v>0.97600399999999998</v>
+        <v>0.97783399999999998</v>
       </c>
       <c r="E21" s="10">
-        <v>0.89062799999999998</v>
+        <v>0.89283699999999999</v>
       </c>
       <c r="F21" s="10">
-        <v>0.97600399999999998</v>
+        <v>0.97783399999999998</v>
       </c>
       <c r="G21" s="10">
-        <v>0.89286500000000002</v>
+        <v>0.88974299999999995</v>
       </c>
       <c r="H21" s="10">
-        <v>0.97600399999999998</v>
+        <v>0.97783399999999998</v>
       </c>
       <c r="I21" s="10">
-        <v>0.89146999999999998</v>
+        <v>0.89097599999999999</v>
       </c>
       <c r="J21" s="10">
-        <v>91.271626999999995</v>
+        <v>95.795636000000002</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -4051,28 +4012,28 @@
         <v>9</v>
       </c>
       <c r="C22" s="10">
-        <v>0.97973399999999999</v>
+        <v>0.98160499999999995</v>
       </c>
       <c r="D22" s="10">
-        <v>0.97973399999999999</v>
+        <v>0.98160499999999995</v>
       </c>
       <c r="E22" s="10">
-        <v>0.89608100000000002</v>
+        <v>0.91627800000000004</v>
       </c>
       <c r="F22" s="10">
-        <v>0.97973399999999999</v>
+        <v>0.98160499999999995</v>
       </c>
       <c r="G22" s="10">
-        <v>0.90986999999999996</v>
+        <v>0.90853499999999998</v>
       </c>
       <c r="H22" s="10">
-        <v>0.97973399999999999</v>
+        <v>0.98160499999999995</v>
       </c>
       <c r="I22" s="10">
-        <v>0.90269100000000002</v>
+        <v>0.91060700000000006</v>
       </c>
       <c r="J22" s="10">
-        <v>91.44162</v>
+        <v>95.937090999999995</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -4080,28 +4041,28 @@
         <v>10</v>
       </c>
       <c r="C23" s="10">
-        <v>0.97894700000000001</v>
+        <v>0.97947700000000004</v>
       </c>
       <c r="D23" s="10">
-        <v>0.97894700000000001</v>
+        <v>0.97947700000000004</v>
       </c>
       <c r="E23" s="10">
-        <v>0.88047500000000001</v>
+        <v>0.89459200000000005</v>
       </c>
       <c r="F23" s="10">
-        <v>0.97894700000000001</v>
+        <v>0.97947700000000004</v>
       </c>
       <c r="G23" s="10">
-        <v>0.93635599999999997</v>
+        <v>0.91717000000000004</v>
       </c>
       <c r="H23" s="10">
-        <v>0.97894700000000001</v>
+        <v>0.97947700000000004</v>
       </c>
       <c r="I23" s="10">
-        <v>0.90686900000000004</v>
+        <v>0.90556800000000004</v>
       </c>
       <c r="J23" s="10">
-        <v>91.230057000000002</v>
+        <v>95.837373999999997</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -4140,102 +4101,102 @@
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="G27" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="J27" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C28" s="7">
         <f>AVERAGE(C14:C23)</f>
-        <v>0.97880869999999986</v>
+        <v>0.97774209999999984</v>
       </c>
       <c r="D28" s="7">
         <f t="shared" ref="D28:J28" si="0">AVERAGE(D14:D23)</f>
-        <v>0.97880869999999986</v>
+        <v>0.97774209999999984</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
-        <v>0.89357580000000014</v>
+        <v>0.88639360000000011</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="0"/>
-        <v>0.97880869999999986</v>
+        <v>0.97774209999999984</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="0"/>
-        <v>0.910134</v>
+        <v>0.91379540000000004</v>
       </c>
       <c r="H28" s="7">
         <f t="shared" si="0"/>
-        <v>0.97880869999999986</v>
+        <v>0.97774209999999984</v>
       </c>
       <c r="I28" s="7">
         <f t="shared" si="0"/>
-        <v>0.90083690000000005</v>
+        <v>0.89830169999999998</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="0"/>
-        <v>93.938391799999977</v>
+        <v>95.376418999999984</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" s="3">
         <f>STDEV(C14:C23)</f>
-        <v>2.6891003472867617E-3</v>
+        <v>2.7544754874769062E-3</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" ref="D29:J29" si="1">STDEV(D14:D23)</f>
-        <v>2.6891003472867617E-3</v>
+        <v>2.7544754874769062E-3</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="1"/>
-        <v>2.0410580561180624E-2</v>
+        <v>2.5425011872388801E-2</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="1"/>
-        <v>2.6891003472867617E-3</v>
+        <v>2.7544754874769062E-3</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>1.4416129300197048E-2</v>
+        <v>1.7781118270045155E-2</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="1"/>
-        <v>2.6891003472867617E-3</v>
+        <v>2.7544754874769062E-3</v>
       </c>
       <c r="I29" s="3">
         <f t="shared" si="1"/>
-        <v>1.0322115636395039E-2</v>
+        <v>1.1193507116479047E-2</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" si="1"/>
-        <v>2.7304627765816871</v>
+        <v>1.4659500375712375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>